<commit_message>
Update results spreadsheet + add feature importance using RF clf
</commit_message>
<xml_diff>
--- a/Results_after_evo_opt.xlsx
+++ b/Results_after_evo_opt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fell\Documents\Studia\Master\sdss-analysis-and-classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2549EF-B1CF-49DC-9DCB-B0F5C44774E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DCFAB5-230B-4A5E-8F84-DEFF77D3C9A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F1235F60-6CD7-426A-AAFE-205D59CA661A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F1235F60-6CD7-426A-AAFE-205D59CA661A}"/>
   </bookViews>
   <sheets>
     <sheet name="acc" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="45">
   <si>
     <t>Classifier</t>
   </si>
@@ -175,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +198,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -241,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -251,6 +259,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2309,6 +2318,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28289956320515697"/>
+          <c:y val="1.6080400313335675E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2795,6 +2812,7 @@
         <c:axId val="1673951247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5194,15 +5212,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5273,7 +5291,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DC8E53B5-6A22-405F-BE2D-04059371297D}" name="Table58" displayName="Table58" ref="S1:S22" totalsRowShown="0">
   <autoFilter ref="S1:S22" xr:uid="{8CE6263B-14B4-4F5F-B004-C7D70C7700E4}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{EA07727C-D767-472A-9E54-8B97C7B4FEB1}" name="Zysk (%)" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{EA07727C-D767-472A-9E54-8B97C7B4FEB1}" name="Zysk (%)" dataDxfId="1">
       <calculatedColumnFormula>(Tabela3[[#This Row],[F1-Score po optymalizacji]]-Tabela3[[#This Row],[F1-Score przed optymalizacją]])*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5324,7 +5342,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{315940B4-0EFE-448E-B444-0BDCDBFB0995}" name="Table57" displayName="Table57" ref="S1:S22" totalsRowShown="0">
   <autoFilter ref="S1:S22" xr:uid="{651ABEAF-8D6C-41E9-BD60-4A9ACC9C1809}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{16F6EE61-00AA-46EE-BBCD-7AD02A64058B}" name="Zysk (%)" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{16F6EE61-00AA-46EE-BBCD-7AD02A64058B}" name="Zysk (%)" dataDxfId="0">
       <calculatedColumnFormula>(Tabela2[[#This Row],[Precyzja po optymalizacji]]-Tabela2[[#This Row],[Precyzja bez optymalizacji]])*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5631,8 +5649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0BEC679-51C9-470B-BD65-9D9A7AA0031A}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5858,7 +5876,7 @@
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>0.990267196326161</v>
       </c>
       <c r="C15">
@@ -5951,7 +5969,7 @@
       <c r="B21">
         <v>0.98880124017832804</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>0.99160035211867403</v>
       </c>
       <c r="J21">
@@ -6292,8 +6310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC459B3-E495-471E-8437-2C6FF18605CF}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6519,7 +6537,7 @@
       <c r="B15">
         <v>0.97947814550366497</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>0.98499374114638905</v>
       </c>
       <c r="S15">
@@ -6606,7 +6624,7 @@
       <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <v>0.983676122235983</v>
       </c>
       <c r="C21">
@@ -6952,8 +6970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481EFA3D-6C9D-46F0-AE54-114DE00621A3}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7192,10 +7210,10 @@
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>0.98387178172451495</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>0.98518930478116795</v>
       </c>
       <c r="S16">
@@ -7611,10 +7629,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF92B79-7168-431E-BE11-8201F4FA7B2A}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7690,7 +7708,7 @@
       <c r="B5">
         <v>0.97674772661366005</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>0.98655164564940001</v>
       </c>
       <c r="S5">
@@ -7927,7 +7945,7 @@
       <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <v>0.98782498161434795</v>
       </c>
       <c r="C21">
@@ -7951,6 +7969,289 @@
       <c r="S22">
         <f>(Tabela2[[#This Row],[Precyzja po optymalizacji]]-Tabela2[[#This Row],[Precyzja bez optymalizacji]])*100</f>
         <v>0.10495377818220408</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.95776086682779205</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.96385991465246368</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.60990478246717739</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1">
+        <v>7.1891780678203883E-3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6.0788155559827117E-3</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.48507932399105319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.96780581332429105</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.97420001380653398</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.10495377818220408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3.2944952680303299E-2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2.7856632420965845E-2</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2.2229127202470096</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.0853699071074236E-3</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7.7599196983680545E-4</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4.9413409618359596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="1">
+        <v>8.6454797842320907E-2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.35738844424230143</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="1">
+        <v>10.656543656035714</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-1.1610557466362306</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="1">
+        <v>-1.333909240232821</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2.9406040699002682</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.104403197508393</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.0336914313304031E-2</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="1">
+        <v>10.653304617469594</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.88342178410595495</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.90621473133609598</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-1.6252703190565931</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.98782498161434795</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.98655164564940001</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="1">
+        <v>9.0280342984130009</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1">
+        <v>20.112978203383634</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="1">
+        <v>20.241058207701737</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="1">
+        <v>12.808000431810726</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="2">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="2">
+        <v>21</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="2">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>